<commit_message>
Implemented Java Document:comment and Testng.xml file
</commit_message>
<xml_diff>
--- a/samadhan_Procurement_Farmer/testData/SamadhanTestData.xlsx
+++ b/samadhan_Procurement_Farmer/testData/SamadhanTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testing.engineer\git\procurement_samadhan\final\samadhan_Procurement_Farmer\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C91E3F-96B9-40DD-B9F4-CEEBDAD96410}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8D0F73-7531-45A0-AD39-A58DBECF0F6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23640" windowHeight="12930" xr2:uid="{2CC6217F-CAE6-4F50-B036-4AB30A51CEFD}"/>
   </bookViews>
@@ -536,6 +536,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f8021fd8-9dec-452d-b422-3220fa843c88" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100237818F2798A2C48BDC4C5150A01F876" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18491cb9e51c5fe50e5ef2e226008270">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f8021fd8-9dec-452d-b422-3220fa843c88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e2b084cb031fe6dfda0f1c80b71eb1f" ns3:_="">
     <xsd:import namespace="f8021fd8-9dec-452d-b422-3220fa843c88"/>
@@ -723,24 +740,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f8021fd8-9dec-452d-b422-3220fa843c88" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773AC705-8959-497F-B233-B518F236F1CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5982256F-B020-44BC-9EA5-A95E177BC1B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f8021fd8-9dec-452d-b422-3220fa843c88"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C540CDA6-FF5F-4710-BDA1-D0E22A382949}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -756,28 +780,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5982256F-B020-44BC-9EA5-A95E177BC1B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f8021fd8-9dec-452d-b422-3220fa843c88"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773AC705-8959-497F-B233-B518F236F1CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>